<commit_message>
"Working on upload to Orchestrator"
</commit_message>
<xml_diff>
--- a/Order Information/JoeyTribbiani_281092.xlsx
+++ b/Order Information/JoeyTribbiani_281092.xlsx
@@ -1,20 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <x:workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hosgo\OneDrive\Documents\UiPath\Invoice Scraping Project\Order Information\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8446CA24-9D4B-4345-944C-4333529BF80E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView firstSheet="0" activeTab="0"/>
+    <x:workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <x:sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </x:sheets>
   <x:definedNames/>
-  <x:calcPr calcId="125725"/>
+  <x:calcPr calcId="0"/>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <x:si>
     <x:t xml:space="preserve">Invoice # 281092 </x:t>
   </x:si>
@@ -198,18 +205,22 @@
   </x:si>
   <x:si>
     <x:t xml:space="preserve">38772.00 </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">HP Laserjet Multifunction Printer B/W (2nd Tray 
+Optional) 
+</x:t>
   </x:si>
 </x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="1">
+  <x:fonts count="1" x14ac:knownFonts="1">
     <x:font>
-      <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color rgb="FF000000"/>
       <x:name val="Calibri"/>
@@ -225,42 +236,35 @@
     </x:fill>
   </x:fills>
   <x:borders count="1">
-    <x:border diagonalUp="0" diagonalDown="0">
-      <x:left style="none">
-        <x:color rgb="FF000000"/>
-      </x:left>
-      <x:right style="none">
-        <x:color rgb="FF000000"/>
-      </x:right>
-      <x:top style="none">
-        <x:color rgb="FF000000"/>
-      </x:top>
-      <x:bottom style="none">
-        <x:color rgb="FF000000"/>
-      </x:bottom>
-      <x:diagonal style="none">
-        <x:color rgb="FF000000"/>
-      </x:diagonal>
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
     </x:border>
   </x:borders>
   <x:cellStyleXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </x:cellStyleXfs>
   <x:cellXfs count="2">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <x:alignment wrapText="1"/>
     </x:xf>
   </x:cellXfs>
   <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </x:ext>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </x:ext>
+  </x:extLst>
 </x:styleSheet>
 </file>
 
@@ -548,27 +552,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:A1"/>
+  <x:dimension ref="A1:E23"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0"/>
+    <x:sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <x:selection activeCell="A23" sqref="A23 23:28"/>
+    </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <x:sheetData>
-    <x:row r="1" spans="1:5">
+    <x:row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:5">
+    <x:row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <x:c r="A2" s="0" t="s">
         <x:v>1</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:5">
+    <x:row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <x:c r="A3" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
@@ -585,7 +591,7 @@
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:5">
+    <x:row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <x:c r="A4" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
@@ -602,7 +608,7 @@
         <x:v>8</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:5">
+    <x:row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <x:c r="A5" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
@@ -619,7 +625,7 @@
         <x:v>11</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:5">
+    <x:row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <x:c r="A6" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -636,7 +642,7 @@
         <x:v>14</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:5">
+    <x:row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <x:c r="A7" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -653,7 +659,7 @@
         <x:v>18</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:5">
+    <x:row r="8" spans="1:5" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A8" s="0" t="s">
         <x:v>19</x:v>
       </x:c>
@@ -670,7 +676,7 @@
         <x:v>21</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="1:5">
+    <x:row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <x:c r="A9" s="0" t="s">
         <x:v>22</x:v>
       </x:c>
@@ -687,7 +693,7 @@
         <x:v>24</x:v>
       </x:c>
     </x:row>
-    <x:row r="10" spans="1:5">
+    <x:row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <x:c r="A10" s="0" t="s">
         <x:v>25</x:v>
       </x:c>
@@ -704,7 +710,7 @@
         <x:v>27</x:v>
       </x:c>
     </x:row>
-    <x:row r="11" spans="1:5">
+    <x:row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <x:c r="A11" s="0" t="s">
         <x:v>28</x:v>
       </x:c>
@@ -721,7 +727,7 @@
         <x:v>24</x:v>
       </x:c>
     </x:row>
-    <x:row r="12" spans="1:5">
+    <x:row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <x:c r="A12" s="0" t="s">
         <x:v>30</x:v>
       </x:c>
@@ -738,7 +744,7 @@
         <x:v>32</x:v>
       </x:c>
     </x:row>
-    <x:row r="13" spans="1:5">
+    <x:row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <x:c r="A13" s="0" t="s">
         <x:v>33</x:v>
       </x:c>
@@ -755,7 +761,7 @@
         <x:v>35</x:v>
       </x:c>
     </x:row>
-    <x:row r="14" spans="1:5">
+    <x:row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <x:c r="A14" s="0" t="s">
         <x:v>36</x:v>
       </x:c>
@@ -772,7 +778,7 @@
         <x:v>38</x:v>
       </x:c>
     </x:row>
-    <x:row r="15" spans="1:5">
+    <x:row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <x:c r="A15" s="0" t="s">
         <x:v>39</x:v>
       </x:c>
@@ -789,7 +795,7 @@
         <x:v>41</x:v>
       </x:c>
     </x:row>
-    <x:row r="16" spans="1:5">
+    <x:row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <x:c r="A16" s="0" t="s">
         <x:v>42</x:v>
       </x:c>
@@ -806,7 +812,7 @@
         <x:v>44</x:v>
       </x:c>
     </x:row>
-    <x:row r="17" spans="1:5">
+    <x:row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <x:c r="A17" s="0" t="s">
         <x:v>45</x:v>
       </x:c>
@@ -823,7 +829,7 @@
         <x:v>24</x:v>
       </x:c>
     </x:row>
-    <x:row r="18" spans="1:5">
+    <x:row r="18" spans="1:5" customFormat="1" ht="129.6" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A18" s="0" t="s">
         <x:v>47</x:v>
       </x:c>
@@ -840,7 +846,7 @@
         <x:v>50</x:v>
       </x:c>
     </x:row>
-    <x:row r="19" spans="1:5">
+    <x:row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <x:c r="A19" s="0" t="s">
         <x:v>51</x:v>
       </x:c>
@@ -857,7 +863,7 @@
         <x:v>53</x:v>
       </x:c>
     </x:row>
-    <x:row r="20" spans="1:5">
+    <x:row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <x:c r="D20" s="0" t="s">
         <x:v>54</x:v>
       </x:c>
@@ -865,7 +871,7 @@
         <x:v>55</x:v>
       </x:c>
     </x:row>
-    <x:row r="21" spans="1:5">
+    <x:row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <x:c r="D21" s="0" t="s">
         <x:v>56</x:v>
       </x:c>
@@ -873,11 +879,69 @@
         <x:v>57</x:v>
       </x:c>
     </x:row>
-    <x:row r="22" spans="1:5">
+    <x:row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <x:c r="D22" s="0" t="s">
         <x:v>58</x:v>
       </x:c>
       <x:c r="E22" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <x:c r="A23" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="B23" s="1" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="C23" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="D23" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="E23" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:5">
+      <x:c r="A24" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="B24" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="C24" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="D24" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="E24" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:5">
+      <x:c r="D25" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="E25" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:5">
+      <x:c r="D26" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="E26" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:5">
+      <x:c r="D27" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="E27" s="0" t="s">
         <x:v>59</x:v>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
"Fix issue with upload to queue Adding Send to mail "
</commit_message>
<xml_diff>
--- a/Order Information/JoeyTribbiani_281092.xlsx
+++ b/Order Information/JoeyTribbiani_281092.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <x:si>
     <x:t xml:space="preserve">Invoice # 281092 </x:t>
   </x:si>
@@ -213,11 +213,6 @@
   </x:si>
   <x:si>
     <x:t xml:space="preserve">38772.00 </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">HP Laserjet Multifunction Printer B/W (2nd Tray 
-Optional) 
-</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -918,64 +913,6 @@
         <x:v>64</x:v>
       </x:c>
     </x:row>
-    <x:row r="24" spans="1:5">
-      <x:c r="A24" s="0" t="s">
-        <x:v>52</x:v>
-      </x:c>
-      <x:c r="B24" s="1" t="s">
-        <x:v>65</x:v>
-      </x:c>
-      <x:c r="C24" s="0" t="s">
-        <x:v>54</x:v>
-      </x:c>
-      <x:c r="D24" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="E24" s="0" t="s">
-        <x:v>55</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="25" spans="1:5">
-      <x:c r="A25" s="0" t="s">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="B25" s="0" t="s">
-        <x:v>57</x:v>
-      </x:c>
-      <x:c r="C25" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D25" s="0" t="s">
-        <x:v>58</x:v>
-      </x:c>
-      <x:c r="E25" s="0" t="s">
-        <x:v>58</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="26" spans="1:5">
-      <x:c r="D26" s="0" t="s">
-        <x:v>59</x:v>
-      </x:c>
-      <x:c r="E26" s="0" t="s">
-        <x:v>60</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="27" spans="1:5">
-      <x:c r="D27" s="0" t="s">
-        <x:v>61</x:v>
-      </x:c>
-      <x:c r="E27" s="0" t="s">
-        <x:v>62</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="28" spans="1:5">
-      <x:c r="D28" s="0" t="s">
-        <x:v>63</x:v>
-      </x:c>
-      <x:c r="E28" s="0" t="s">
-        <x:v>64</x:v>
-      </x:c>
-    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>